<commit_message>
added Macro random assignment component-wise
</commit_message>
<xml_diff>
--- a/V1_BG_Thal_V1_Loop.xlsx
+++ b/V1_BG_Thal_V1_Loop.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nightcrawler/Dropbox/AllenBrain_SNMC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{491B9EF6-151A-3C4B-9341-EF439DC6351C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9161D1F8-01FD-FD44-A872-44BBF5A308DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" activeTab="2" xr2:uid="{3E99C6B3-0F65-5241-BE7A-90D3895F20C9}"/>
+    <workbookView xWindow="3160" yWindow="1380" windowWidth="33260" windowHeight="18420" activeTab="1" xr2:uid="{3E99C6B3-0F65-5241-BE7A-90D3895F20C9}"/>
   </bookViews>
   <sheets>
     <sheet name="RawInjectionData" sheetId="1" r:id="rId1"/>
@@ -6141,8 +6141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12A7426A-06CD-2A46-805E-0167ED4E08CB}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6152,7 +6152,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>273</v>
       </c>
       <c r="B1" t="s">
         <v>87</v>
@@ -6327,7 +6327,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D60CBBD5-77FA-C849-9426-BEC279FEC31F}">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
finished macro random assignment functions
</commit_message>
<xml_diff>
--- a/V1_BG_Thal_V1_Loop.xlsx
+++ b/V1_BG_Thal_V1_Loop.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nightcrawler/Dropbox/AllenBrain_SNMC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9161D1F8-01FD-FD44-A872-44BBF5A308DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73374C49-4349-8740-ACAC-3A3E3A894288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3160" yWindow="1380" windowWidth="33260" windowHeight="18420" activeTab="1" xr2:uid="{3E99C6B3-0F65-5241-BE7A-90D3895F20C9}"/>
+    <workbookView xWindow="29920" yWindow="500" windowWidth="50880" windowHeight="18200" activeTab="1" xr2:uid="{3E99C6B3-0F65-5241-BE7A-90D3895F20C9}"/>
   </bookViews>
   <sheets>
     <sheet name="RawInjectionData" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1252" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1261" uniqueCount="288">
   <si>
     <t>grey</t>
   </si>
@@ -892,6 +892,33 @@
   </si>
   <si>
     <t>L2Vip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">note a tiny bit of anterior cortex gets hit (image 41). This is probably the source of the isocortex signal. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">there is no SSbfd or V1 signal…the numbers in the isocortex header are .0002 or less except where the off site injection is. </t>
+  </si>
+  <si>
+    <t>SSbfd and V1 less than .0001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None of the cortex is actually hit it seems.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This LD injection hits both S1 and V1 (also RS) and that's basically it. That's pretty amazing considering their cortical interconnection. </t>
+  </si>
+  <si>
+    <t>Just use total V1 here because the layer analysis is clearly wrong. On slide 82-91 it is basically all L4 in V1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The V1 is no doubt real and strong. The S1 is located way way down on the bottom of Layer 6, and likely </t>
+  </si>
+  <si>
+    <t xml:space="preserve">not layer 6 (probably CC, not terminating). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interestingly, I would also say that the CP signal is all fibers of passage. (see image 63). There are no clear terminals. </t>
   </si>
 </sst>
 </file>
@@ -1314,8 +1341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF0D635E-52FA-FB44-B276-339BA8083DF4}">
   <dimension ref="A1:K263"/>
   <sheetViews>
-    <sheetView topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="D145" sqref="D145"/>
+    <sheetView topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="K83" sqref="K83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2165,7 +2192,9 @@
       <c r="J29" t="s">
         <v>115</v>
       </c>
-      <c r="K29" s="1"/>
+      <c r="K29" s="1" t="s">
+        <v>279</v>
+      </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
@@ -2194,7 +2223,9 @@
       <c r="J30" t="s">
         <v>115</v>
       </c>
-      <c r="K30" s="1"/>
+      <c r="K30" s="1" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
@@ -2685,7 +2716,9 @@
       <c r="J47" t="s">
         <v>116</v>
       </c>
-      <c r="K47" s="1"/>
+      <c r="K47" s="1" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
@@ -2712,7 +2745,9 @@
       <c r="J48" t="s">
         <v>116</v>
       </c>
-      <c r="K48" s="1"/>
+      <c r="K48" s="1" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
@@ -3133,7 +3168,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>35</v>
       </c>
@@ -3159,7 +3194,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>37</v>
       </c>
@@ -3185,7 +3220,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>38</v>
       </c>
@@ -3211,7 +3246,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>50</v>
       </c>
@@ -3237,7 +3272,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>39</v>
       </c>
@@ -3263,7 +3298,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>68</v>
       </c>
@@ -3289,7 +3324,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>69</v>
       </c>
@@ -3315,7 +3350,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>40</v>
       </c>
@@ -3341,7 +3376,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>42</v>
       </c>
@@ -3367,7 +3402,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>70</v>
       </c>
@@ -3393,7 +3428,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>71</v>
       </c>
@@ -3419,7 +3454,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>72</v>
       </c>
@@ -3445,7 +3480,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>73</v>
       </c>
@@ -3473,7 +3508,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" s="5" t="s">
         <v>0</v>
       </c>
@@ -3500,8 +3535,11 @@
       <c r="J78" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K78" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" s="5" t="s">
         <v>1</v>
       </c>
@@ -3528,8 +3566,11 @@
       <c r="J79" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K79" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" s="5" t="s">
         <v>47</v>
       </c>
@@ -3556,8 +3597,11 @@
       <c r="J80" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K80" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" s="5" t="s">
         <v>46</v>
       </c>
@@ -3584,8 +3628,11 @@
       <c r="J81" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K81" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" s="5" t="s">
         <v>76</v>
       </c>
@@ -3613,7 +3660,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" s="5" t="s">
         <v>77</v>
       </c>
@@ -3640,8 +3687,11 @@
       <c r="J83" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K83" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" s="5" t="s">
         <v>2</v>
       </c>
@@ -3669,7 +3719,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" s="5" t="s">
         <v>3</v>
       </c>
@@ -3697,7 +3747,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" s="5" t="s">
         <v>22</v>
       </c>
@@ -3725,7 +3775,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" s="5" t="s">
         <v>23</v>
       </c>
@@ -3753,7 +3803,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" s="5" t="s">
         <v>24</v>
       </c>
@@ -3781,7 +3831,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" s="5" t="s">
         <v>25</v>
       </c>
@@ -3809,7 +3859,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" s="5" t="s">
         <v>26</v>
       </c>
@@ -3837,7 +3887,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" s="5" t="s">
         <v>27</v>
       </c>
@@ -3865,7 +3915,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" s="5" t="s">
         <v>4</v>
       </c>
@@ -3893,7 +3943,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" s="5" t="s">
         <v>5</v>
       </c>
@@ -3921,7 +3971,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" s="5" t="s">
         <v>6</v>
       </c>
@@ -3949,7 +3999,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" s="5" t="s">
         <v>78</v>
       </c>
@@ -3977,7 +4027,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" s="5" t="s">
         <v>57</v>
       </c>
@@ -6142,7 +6192,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6190,7 +6240,9 @@
       <c r="E2" s="5">
         <v>0</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="F2" s="5">
+        <v>0</v>
+      </c>
       <c r="G2" t="s">
         <v>89</v>
       </c>
@@ -6211,6 +6263,9 @@
       <c r="E3">
         <v>7.7999999999999996E-3</v>
       </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
       <c r="G3" t="s">
         <v>89</v>
       </c>
@@ -6232,7 +6287,9 @@
         <v>0</v>
       </c>
       <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
+      <c r="F4" s="5">
+        <v>5.7999999999999996E-3</v>
+      </c>
       <c r="G4" t="s">
         <v>89</v>
       </c>

</xml_diff>

<commit_message>
Finished commenting synapse connectivity
</commit_message>
<xml_diff>
--- a/V1_BG_Thal_V1_Loop.xlsx
+++ b/V1_BG_Thal_V1_Loop.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nightcrawler/Dropbox/AllenBrain_SNMC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73374C49-4349-8740-ACAC-3A3E3A894288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3CBC8F4F-8C67-0E43-8A7C-AEE4F0070CE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29920" yWindow="500" windowWidth="50880" windowHeight="18200" activeTab="1" xr2:uid="{3E99C6B3-0F65-5241-BE7A-90D3895F20C9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" xr2:uid="{3E99C6B3-0F65-5241-BE7A-90D3895F20C9}"/>
   </bookViews>
   <sheets>
     <sheet name="RawInjectionData" sheetId="1" r:id="rId1"/>
-    <sheet name="longrange_FINAL" sheetId="2" r:id="rId2"/>
+    <sheet name="longrange" sheetId="2" r:id="rId2"/>
     <sheet name="v1mouse" sheetId="7" r:id="rId3"/>
     <sheet name="PairwiseMicrocolumnConnections" sheetId="3" r:id="rId4"/>
     <sheet name="microcircuit_probabilities" sheetId="4" r:id="rId5"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1261" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1264" uniqueCount="291">
   <si>
     <t>grey</t>
   </si>
@@ -920,12 +920,21 @@
   <si>
     <t xml:space="preserve">Interestingly, I would also say that the CP signal is all fibers of passage. (see image 63). There are no clear terminals. </t>
   </si>
+  <si>
+    <t>S1 L5</t>
+  </si>
+  <si>
+    <t>S1 L234</t>
+  </si>
+  <si>
+    <t>CP at S1 terminals (opp hemisphere)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -988,6 +997,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1010,7 +1026,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -1024,6 +1040,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1341,8 +1358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF0D635E-52FA-FB44-B276-339BA8083DF4}">
   <dimension ref="A1:K263"/>
   <sheetViews>
-    <sheetView topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="K83" sqref="K83"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="G84" sqref="G84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5393,6 +5410,12 @@
       <c r="C146" s="1"/>
       <c r="D146" s="1"/>
       <c r="E146" s="1"/>
+      <c r="G146">
+        <v>643749624</v>
+      </c>
+      <c r="H146" t="s">
+        <v>288</v>
+      </c>
       <c r="I146" s="1"/>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.2">
@@ -5401,6 +5424,12 @@
       <c r="C147" s="1"/>
       <c r="D147" s="1"/>
       <c r="E147" s="1"/>
+      <c r="G147" s="9">
+        <v>266486371</v>
+      </c>
+      <c r="H147" t="s">
+        <v>289</v>
+      </c>
       <c r="I147" s="1"/>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.2">
@@ -5409,6 +5438,12 @@
       <c r="C148" s="1"/>
       <c r="D148" s="1"/>
       <c r="E148" s="1"/>
+      <c r="G148">
+        <v>100142580</v>
+      </c>
+      <c r="H148" t="s">
+        <v>290</v>
+      </c>
       <c r="I148" s="1"/>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.2">
@@ -6191,8 +6226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12A7426A-06CD-2A46-805E-0167ED4E08CB}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>